<commit_message>
Projekt-Demo PDF-Datei wurde hochgeladen
</commit_message>
<xml_diff>
--- a/Data/Student Mandatory Modules Grades Data.xlsx
+++ b/Data/Student Mandatory Modules Grades Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_Projekte\OptiModuls_MP_87\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA5CFDA-63CD-4D6C-AFC3-B7212AB56B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F707BF-2FB4-4A8A-BECA-1140D391DBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -702,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1919,82 +1919,82 @@
         <v>5000014</v>
       </c>
       <c r="E15">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="F15">
+        <v>95</v>
+      </c>
+      <c r="G15">
+        <v>100</v>
+      </c>
+      <c r="H15">
+        <v>94</v>
+      </c>
+      <c r="I15">
+        <v>73</v>
+      </c>
+      <c r="J15">
+        <v>81</v>
+      </c>
+      <c r="K15">
+        <v>77</v>
+      </c>
+      <c r="L15">
+        <v>73</v>
+      </c>
+      <c r="M15">
+        <v>70</v>
+      </c>
+      <c r="N15">
         <v>80</v>
       </c>
-      <c r="G15">
-        <v>95</v>
-      </c>
-      <c r="H15">
-        <v>79</v>
-      </c>
-      <c r="I15">
-        <v>58</v>
-      </c>
-      <c r="J15">
+      <c r="O15">
+        <v>73</v>
+      </c>
+      <c r="P15">
+        <v>67</v>
+      </c>
+      <c r="Q15">
+        <v>85</v>
+      </c>
+      <c r="R15">
+        <v>98</v>
+      </c>
+      <c r="S15">
+        <v>100</v>
+      </c>
+      <c r="T15">
+        <v>86</v>
+      </c>
+      <c r="U15">
+        <v>88</v>
+      </c>
+      <c r="V15">
         <v>66</v>
       </c>
-      <c r="K15">
-        <v>62</v>
-      </c>
-      <c r="L15">
-        <v>58</v>
-      </c>
-      <c r="M15">
-        <v>55</v>
-      </c>
-      <c r="N15">
+      <c r="W15">
+        <v>75</v>
+      </c>
+      <c r="X15">
         <v>65</v>
       </c>
-      <c r="O15">
-        <v>58</v>
-      </c>
-      <c r="P15">
-        <v>52</v>
-      </c>
-      <c r="Q15">
-        <v>70</v>
-      </c>
-      <c r="R15">
-        <v>83</v>
-      </c>
-      <c r="S15">
-        <v>86</v>
-      </c>
-      <c r="T15">
-        <v>71</v>
-      </c>
-      <c r="U15">
-        <v>73</v>
-      </c>
-      <c r="V15">
-        <v>51</v>
-      </c>
-      <c r="W15">
-        <v>60</v>
-      </c>
-      <c r="X15">
-        <v>50</v>
-      </c>
       <c r="Y15">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="Z15">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="AA15">
+        <v>82</v>
+      </c>
+      <c r="AB15">
         <v>67</v>
       </c>
-      <c r="AB15">
-        <v>52</v>
-      </c>
       <c r="AC15">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="AD15">
-        <v>66</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>